<commit_message>
Export smets to excel with indexes of Department and Category
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8221B1-FE2B-4DAF-BB18-C9F9B39687C5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBAE0C3-2B29-420D-9AF8-AB8A1127C76C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10770" yWindow="465" windowWidth="16440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" fullCalcOnLoad="1"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Cмета проекта</t>
   </si>
@@ -74,32 +74,13 @@
   </si>
   <si>
     <t>Головы/Moving heads</t>
-  </si>
-  <si>
-    <t>Clay Paky Alpha Beam 1500</t>
-  </si>
-  <si>
-    <t>Clay Paky Alpha Profile 1500</t>
-  </si>
-  <si>
-    <t>Skylight F230</t>
-  </si>
-  <si>
-    <t>Esdelumen Smart p6.0 0.576 x0.576m, 96x96 pixels, 0.25 sq.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ферма  треугольная/truss triangle 30х30, 2м (стрелы)</t>
-  </si>
-  <si>
-    <t>кубы 30х30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,98 +301,96 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="4" applyFill="1" borderId="6" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="8" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Обычный 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -738,16 +717,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A37" sqref="A10:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="1" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -759,164 +737,133 @@
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="5"/>
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="3"/>
     </row>
-    <row r="2" ht="26.25">
-      <c r="C2" s="20" t="s">
+    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
-    <row r="3" ht="15.75">
-      <c r="C3" s="21" t="s">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="21"/>
+      <c r="J3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="24"/>
+      <c r="K3" s="22"/>
     </row>
-    <row r="4" ht="15.75">
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
-    <row r="5" ht="15.75">
-      <c r="C5" s="17" t="s">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="J5" s="25" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="J5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="24"/>
+      <c r="K5" s="22"/>
     </row>
-    <row r="7" ht="36">
-      <c r="C7" s="9" t="s">
+    <row r="7" spans="1:13" ht="36" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" ht="17.25">
-      <c r="C8" s="18" t="s">
+    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
     </row>
-    <row r="9">
-      <c r="C9" s="19" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <v>0</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="17">
         <v>0</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="C10" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16"/>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="8">
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C2:M2"/>
@@ -933,7 +880,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First export to excel file.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -1,19 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20907"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7602CB-0100-4E06-AA5C-DFB19B7D1939}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8221B1-FE2B-4DAF-BB18-C9F9B39687C5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Cмета проекта</t>
   </si>
@@ -37,15 +34,15 @@
     <t>Контакты</t>
   </si>
   <si>
+    <t xml:space="preserve">Смета составлена в </t>
+  </si>
+  <si>
+    <t>безналичных белорусских рублях без НДС</t>
+  </si>
+  <si>
     <t>+375 29 11 98 025</t>
   </si>
   <si>
-    <t xml:space="preserve">Смета составлена в </t>
-  </si>
-  <si>
-    <t>безналичных белорусских рублях без НДС</t>
-  </si>
-  <si>
     <t>Наименование, name</t>
   </si>
   <si>
@@ -77,13 +74,32 @@
   </si>
   <si>
     <t>Головы/Moving heads</t>
+  </si>
+  <si>
+    <t>Clay Paky Alpha Beam 1500</t>
+  </si>
+  <si>
+    <t>Clay Paky Alpha Profile 1500</t>
+  </si>
+  <si>
+    <t>Skylight F230</t>
+  </si>
+  <si>
+    <t>Esdelumen Smart p6.0 0.576 x0.576m, 96x96 pixels, 0.25 sq.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ферма  треугольная/truss triangle 30х30, 2м (стрелы)</t>
+  </si>
+  <si>
+    <t>кубы 30х30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,14 +126,12 @@
       <color theme="1"/>
       <name val="Segoe UI Semibold"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,21 +146,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFFF6600"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -154,7 +165,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -307,99 +317,101 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="27">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="3" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="4" applyFill="1" borderId="6" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="8" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{C0F8A0ED-C6CA-4DB9-BEAC-8DA9B4FB212C}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{68423C64-64C1-4BDA-8BE8-CD9C1D77D627}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Обычный 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,7 +439,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>703662</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>13032</xdr:rowOff>
+      <xdr:rowOff>13031</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -461,42 +473,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Свет"/>
-      <sheetName val="Экран"/>
-      <sheetName val="Коммутация"/>
-      <sheetName val="Фермы. моторы"/>
-      <sheetName val="Конструктив"/>
-      <sheetName val="Звук"/>
-      <sheetName val="Смета"/>
-      <sheetName val="Персонал,транспорт и пр"/>
-      <sheetName val="ТехЛист"/>
-      <sheetName val="Погрузка"/>
-      <sheetName val="Склад"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="PrintSmeta"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -762,15 +738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -782,133 +759,164 @@
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="C2" s="5" t="s">
+    <row r="1" ht="15.75">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" ht="26.25">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="6" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+    </row>
+    <row r="3" ht="15.75">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="11" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" ht="15.75">
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="24" t="s">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" ht="15.75">
+      <c r="C5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="J5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="J5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="7" spans="1:13" ht="36" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+      <c r="K5" s="24"/>
+    </row>
+    <row r="7" ht="36">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C8" s="20" t="s">
+    <row r="8" ht="17.25">
+      <c r="C8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="21" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9">
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="19">
         <v>0</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>0</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="19">
         <v>0</v>
       </c>
     </row>
+    <row r="10">
+      <c r="C10" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C2:M2"/>
@@ -924,7 +932,8 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made DepartmentName,making CategoryName.Status OK.
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBAE0C3-2B29-420D-9AF8-AB8A1127C76C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14F237A-0A69-4A49-9F14-AFF0061E8112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10770" yWindow="465" windowWidth="16440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7890" yWindow="90" windowWidth="14400" windowHeight="15630" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
+    <sheet name="Serv" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
   <si>
     <t>Cмета проекта</t>
   </si>
@@ -74,13 +75,163 @@
   </si>
   <si>
     <t>Головы/Moving heads</t>
+  </si>
+  <si>
+    <t>Коммутация / Commutation</t>
+  </si>
+  <si>
+    <t>Фермы. Моторы</t>
+  </si>
+  <si>
+    <t>Конструктив</t>
+  </si>
+  <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
+  </si>
+  <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
+    <t>Коммутация/Commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
+    <t>Пары, блайндера/PAR's, blinders</t>
+  </si>
+  <si>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>Архитектурный свет/Architecture fixtures</t>
+  </si>
+  <si>
+    <t>Прочее/rest equipment</t>
+  </si>
+  <si>
+    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
+  </si>
+  <si>
+    <t>Светодиодные приборы/LED fixtures</t>
+  </si>
+  <si>
+    <t>Проектора и проекционные экраны / Projectors and screens</t>
+  </si>
+  <si>
+    <t>Оборудование для подвесса/Rigging stuff</t>
+  </si>
+  <si>
+    <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
+  </si>
+  <si>
+    <t>Экранный конструктив/ Screen construction</t>
+  </si>
+  <si>
+    <t>разное/different stuff</t>
+  </si>
+  <si>
+    <t>Звуковое оборудование / Sound equipment</t>
+  </si>
+  <si>
+    <t>Пульты/lighting desks</t>
+  </si>
+  <si>
+    <t>Цельные конструкции/Complete construction</t>
+  </si>
+  <si>
+    <t>Системы связи/Intercoms and radios</t>
+  </si>
+  <si>
+    <t>Камеры, тв микшера / Cameras, mixing desks</t>
+  </si>
+  <si>
+    <t>Лифты / Stagelifts</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
+  </si>
+  <si>
+    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
+  </si>
+  <si>
+    <t>Разное / different details</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
+    <t>Мониторы / monitors</t>
+  </si>
+  <si>
+    <t>Микшерные пульты / mixing desks</t>
+  </si>
+  <si>
+    <t>dj-оборудование / dj equipment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +310,13 @@
       <i/>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -301,7 +459,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -353,6 +511,10 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -392,7 +554,37 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="3" tint="0.79998168889431442"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -452,6 +644,77 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E34F082-8D24-4A66-BF8B-1BCBC0325CAF}" name="Department" displayName="Department" ref="A1:B8" totalsRowShown="0">
+  <autoFilter ref="A1:B8" xr:uid="{455E10E6-38D2-42A6-BDAF-3E50768603C5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E1880057-F406-470F-960A-B203F61F3487}" name="id_Dep"/>
+    <tableColumn id="2" xr3:uid="{A6814A4F-DCDC-40D6-BEC7-BF0AF871D660}" name="Dep_Name" dataDxfId="0" dataCellStyle="Normal 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{350F0A72-FD54-4B0F-A922-57166741355C}" name="id_Dep_1" displayName="id_Dep_1" ref="E1:E9" totalsRowShown="0">
+  <autoFilter ref="E1:E9" xr:uid="{4E4D8259-88D6-460E-98FD-E82922679913}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{A433C8DB-3BE0-4C7E-A5DB-CD94B32B2B7D}" name="id_Dep_1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C570EA9B-994F-4505-862A-D3EDDAD2961E}" name="id_Dep_2" displayName="id_Dep_2" ref="H1:H9" totalsRowShown="0">
+  <autoFilter ref="H1:H9" xr:uid="{F70E84A7-6453-4423-A35F-FBABF4CFE974}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{9129FF03-88E9-4C6D-A2D3-0FD9CB8BE042}" name="id_Dep_2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D546D0E4-8F35-4B5F-A7B4-7842B9D9F751}" name="id_Dep_3" displayName="id_Dep_3" ref="K1:K5" totalsRowShown="0">
+  <autoFilter ref="K1:K5" xr:uid="{84E4A641-D71E-4C54-ACF9-42C41F12A900}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{0DA3EEDB-6BB6-415D-A520-E5B2A2E66BEB}" name="id_Dep_3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{33C4DC0E-0986-488F-9ED4-3B2AB5DFC61C}" name="id_Dep_4" displayName="id_Dep_4" ref="N1:N9" totalsRowShown="0">
+  <autoFilter ref="N1:N9" xr:uid="{3A1F215E-B6F7-4B45-AC2E-8EAEB54DE869}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{AECFDEBE-0730-4170-8447-89B422DA03A3}" name="id_Dep_4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{457BFFF2-0FF4-4E24-B57E-894E4DBA1A22}" name="id_Dep_5" displayName="id_Dep_5" ref="Q1:Q7" totalsRowShown="0">
+  <autoFilter ref="Q1:Q7" xr:uid="{571ED648-C72E-4894-808E-20828C9BCA89}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{FFE1CB79-0083-4F42-8463-B84E502F4BD1}" name="id_Dep_5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{173D89E3-34D7-4119-8158-0602553D73B1}" name="id_Dep_6" displayName="id_Dep_6" ref="T1:T6" totalsRowShown="0">
+  <autoFilter ref="T1:T6" xr:uid="{5A70343F-EF27-42E5-9F07-1B695B1864C3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{A3E7E8D4-313F-4F0C-83A9-AE127B3C2DD3}" name="id_Dep_6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -719,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A37" sqref="A10:C37"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,36 +1016,36 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="20" t="s">
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="22"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="13"/>
@@ -799,16 +1062,16 @@
       <c r="C5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="J5" s="23" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="J5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="22"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="7" spans="1:13" ht="36" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
@@ -840,25 +1103,25 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="19">
         <v>0</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="19">
         <v>0</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="19">
         <v>0</v>
       </c>
     </row>
@@ -882,4 +1145,273 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E07D3C-DC55-452E-B0EB-BD6DE05EFA5C}">
+  <dimension ref="A1:T22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="33.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="7">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished with Departments and Categories.Next step is format xlSmeta
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14F237A-0A69-4A49-9F14-AFF0061E8112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB5C94-6E57-4AA5-B455-998616341BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="90" windowWidth="14400" windowHeight="15630" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10770" yWindow="465" windowWidth="16440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -77,111 +77,144 @@
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>Пары, блайндера/PAR's, blinders</t>
+  </si>
+  <si>
+    <t>Светодиодные приборы/LED fixtures</t>
+  </si>
+  <si>
+    <t>Пульты/lighting desks</t>
+  </si>
+  <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Экранный конструктив/ Screen construction</t>
+  </si>
+  <si>
     <t>Коммутация / Commutation</t>
   </si>
   <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
     <t>Фермы. Моторы</t>
   </si>
   <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
+    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
+  </si>
+  <si>
+    <t>Коммутация/Commutation</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
+  </si>
+  <si>
+    <t>Мониторы / monitors</t>
+  </si>
+  <si>
+    <t>Архитектурный свет/Architecture fixtures</t>
+  </si>
+  <si>
+    <t>Прочее/rest equipment</t>
+  </si>
+  <si>
+    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
+  </si>
+  <si>
+    <t>Микшерные пульты / mixing desks</t>
+  </si>
+  <si>
+    <t>Проектора и проекционные экраны / Projectors and screens</t>
+  </si>
+  <si>
+    <t>Оборудование для подвесса/Rigging stuff</t>
+  </si>
+  <si>
+    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
+  </si>
+  <si>
+    <t>dj-оборудование / dj equipment</t>
+  </si>
+  <si>
     <t>Конструктив</t>
   </si>
   <si>
-    <t>id_Dep</t>
-  </si>
-  <si>
-    <t>Dep_Name</t>
-  </si>
-  <si>
-    <t>id_Dep_1</t>
-  </si>
-  <si>
-    <t>id_Dep_2</t>
-  </si>
-  <si>
-    <t>id_Dep_3</t>
-  </si>
-  <si>
-    <t>id_Dep_4</t>
-  </si>
-  <si>
-    <t>id_Dep_5</t>
-  </si>
-  <si>
-    <t>id_Dep_6</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Screen modules / Модупи экраны</t>
-  </si>
-  <si>
-    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
-  </si>
-  <si>
-    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
-  </si>
-  <si>
-    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
-  </si>
-  <si>
-    <t>Media servers / Медиасервера</t>
-  </si>
-  <si>
-    <t>Коммутация/Commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 40x40</t>
-  </si>
-  <si>
-    <t>Экраны, медиасервера / Screens, mediaservers</t>
-  </si>
-  <si>
-    <t>Пары, блайндера/PAR's, blinders</t>
-  </si>
-  <si>
-    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
-  </si>
-  <si>
-    <t>Силовая коммутация/power commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
-  </si>
-  <si>
-    <t>Архитектурный свет/Architecture fixtures</t>
-  </si>
-  <si>
-    <t>Прочее/rest equipment</t>
-  </si>
-  <si>
-    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
-  </si>
-  <si>
-    <t>Светодиодные приборы/LED fixtures</t>
-  </si>
-  <si>
-    <t>Проектора и проекционные экраны / Projectors and screens</t>
-  </si>
-  <si>
-    <t>Оборудование для подвесса/Rigging stuff</t>
-  </si>
-  <si>
     <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
   </si>
   <si>
-    <t>Экранный конструктив/ Screen construction</t>
-  </si>
-  <si>
     <t>разное/different stuff</t>
   </si>
   <si>
+    <t>Разное / different details</t>
+  </si>
+  <si>
     <t>Звуковое оборудование / Sound equipment</t>
   </si>
   <si>
-    <t>Пульты/lighting desks</t>
-  </si>
-  <si>
     <t>Цельные конструкции/Complete construction</t>
   </si>
   <si>
@@ -192,39 +225,6 @@
   </si>
   <si>
     <t>Лифты / Stagelifts</t>
-  </si>
-  <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
-  </si>
-  <si>
-    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
-  </si>
-  <si>
-    <t>Разное / different details</t>
-  </si>
-  <si>
-    <t>Акустические системы / speakers</t>
-  </si>
-  <si>
-    <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>Мониторы / monitors</t>
-  </si>
-  <si>
-    <t>Микшерные пульты / mixing desks</t>
-  </si>
-  <si>
-    <t>dj-оборудование / dj equipment</t>
   </si>
 </sst>
 </file>
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E07D3C-DC55-452E-B0EB-BD6DE05EFA5C}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -1169,28 +1169,28 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="N1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="T1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1198,25 +1198,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
       <c r="Q2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1229,24 +1229,24 @@
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="T3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1254,25 +1254,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="T4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1280,25 +1280,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="Q5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="T5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1306,22 +1306,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N6" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="Q6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="T6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1329,16 +1329,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="Q7" t="s">
         <v>62</v>
@@ -1349,27 +1349,27 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="N8" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="21" x14ac:dyDescent="0.25">
@@ -1379,27 +1379,27 @@
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="16" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="16" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B22" s="16" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost finished with excelSmeta.Have to format data,create discount and personnel.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB5C94-6E57-4AA5-B455-998616341BF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB55BC7-C06D-4A70-9B67-693F34069FAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10770" yWindow="465" windowWidth="16440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="495" windowWidth="16440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Cмета проекта</t>
   </si>
@@ -44,175 +44,148 @@
     <t>+375 29 11 98 025</t>
   </si>
   <si>
-    <t>Наименование, name</t>
-  </si>
-  <si>
-    <t>Кол-во всего, qtt</t>
-  </si>
-  <si>
-    <t>Вес, weight</t>
-  </si>
-  <si>
-    <t>Мощность, power</t>
-  </si>
-  <si>
-    <t>Вес общ, weight total</t>
-  </si>
-  <si>
-    <t>заказанное кол-во, to take</t>
-  </si>
-  <si>
-    <t>Резерв</t>
-  </si>
-  <si>
-    <t>аренда 1 прибора, price per unit</t>
-  </si>
-  <si>
-    <t>Стоимость общая, total cost</t>
-  </si>
-  <si>
     <t>Световое оборудование/Lighting equipment</t>
   </si>
   <si>
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
+    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
+  </si>
+  <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
+    <t>Коммутация/Commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
     <t>Пары, блайндера/PAR's, blinders</t>
   </si>
   <si>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
+  </si>
+  <si>
+    <t>Мониторы / monitors</t>
+  </si>
+  <si>
+    <t>Коммутация / Commutation</t>
+  </si>
+  <si>
+    <t>Архитектурный свет/Architecture fixtures</t>
+  </si>
+  <si>
+    <t>Прочее/rest equipment</t>
+  </si>
+  <si>
+    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
+  </si>
+  <si>
+    <t>Микшерные пульты / mixing desks</t>
+  </si>
+  <si>
+    <t>Фермы. Моторы</t>
+  </si>
+  <si>
     <t>Светодиодные приборы/LED fixtures</t>
   </si>
   <si>
+    <t>Проектора и проекционные экраны / Projectors and screens</t>
+  </si>
+  <si>
+    <t>Оборудование для подвесса/Rigging stuff</t>
+  </si>
+  <si>
+    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
+  </si>
+  <si>
+    <t>dj-оборудование / dj equipment</t>
+  </si>
+  <si>
+    <t>Конструктив</t>
+  </si>
+  <si>
+    <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
+  </si>
+  <si>
+    <t>Экранный конструктив/ Screen construction</t>
+  </si>
+  <si>
+    <t>разное/different stuff</t>
+  </si>
+  <si>
+    <t>Разное / different details</t>
+  </si>
+  <si>
+    <t>Звуковое оборудование / Sound equipment</t>
+  </si>
+  <si>
     <t>Пульты/lighting desks</t>
-  </si>
-  <si>
-    <t>Экраны, медиасервера / Screens, mediaservers</t>
-  </si>
-  <si>
-    <t>Screen modules / Модупи экраны</t>
-  </si>
-  <si>
-    <t>Media servers / Медиасервера</t>
-  </si>
-  <si>
-    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
-  </si>
-  <si>
-    <t>Экранный конструктив/ Screen construction</t>
-  </si>
-  <si>
-    <t>Коммутация / Commutation</t>
-  </si>
-  <si>
-    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
-  </si>
-  <si>
-    <t>Силовая коммутация/power commutation</t>
-  </si>
-  <si>
-    <t>Фермы. Моторы</t>
-  </si>
-  <si>
-    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
-  </si>
-  <si>
-    <t>Фермы/truss 40x40</t>
-  </si>
-  <si>
-    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
-  </si>
-  <si>
-    <t>id_Dep</t>
-  </si>
-  <si>
-    <t>Dep_Name</t>
-  </si>
-  <si>
-    <t>id_Dep_1</t>
-  </si>
-  <si>
-    <t>id_Dep_2</t>
-  </si>
-  <si>
-    <t>id_Dep_3</t>
-  </si>
-  <si>
-    <t>id_Dep_4</t>
-  </si>
-  <si>
-    <t>id_Dep_5</t>
-  </si>
-  <si>
-    <t>id_Dep_6</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
-    <t>Акустические системы / speakers</t>
-  </si>
-  <si>
-    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
-  </si>
-  <si>
-    <t>Коммутация/Commutation</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
-  </si>
-  <si>
-    <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
-  </si>
-  <si>
-    <t>Мониторы / monitors</t>
-  </si>
-  <si>
-    <t>Архитектурный свет/Architecture fixtures</t>
-  </si>
-  <si>
-    <t>Прочее/rest equipment</t>
-  </si>
-  <si>
-    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
-  </si>
-  <si>
-    <t>Микшерные пульты / mixing desks</t>
-  </si>
-  <si>
-    <t>Проектора и проекционные экраны / Projectors and screens</t>
-  </si>
-  <si>
-    <t>Оборудование для подвесса/Rigging stuff</t>
-  </si>
-  <si>
-    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
-  </si>
-  <si>
-    <t>dj-оборудование / dj equipment</t>
-  </si>
-  <si>
-    <t>Конструктив</t>
-  </si>
-  <si>
-    <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
-  </si>
-  <si>
-    <t>разное/different stuff</t>
-  </si>
-  <si>
-    <t>Разное / different details</t>
-  </si>
-  <si>
-    <t>Звуковое оборудование / Sound equipment</t>
   </si>
   <si>
     <t>Цельные конструкции/Complete construction</t>
@@ -231,7 +204,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,60 +241,13 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF6600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF002060"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,20 +260,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F5F5"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -406,28 +320,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </left>
-      <right style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="3" tint="0.79998168889431442"/>
       </bottom>
@@ -437,19 +332,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="3" tint="0.79998168889431442"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -459,7 +345,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -481,24 +367,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -507,20 +375,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,7 +407,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -586,6 +453,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF2F2F5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -601,16 +473,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>703662</xdr:colOff>
+      <xdr:colOff>944962</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>13031</xdr:rowOff>
+      <xdr:rowOff>178130</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -633,8 +505,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="241300" y="38100"/>
-          <a:ext cx="944962" cy="914732"/>
+          <a:off x="482600" y="203200"/>
+          <a:ext cx="944962" cy="914731"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -980,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,9 +866,10 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="12" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="12" width="12.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1016,119 +889,67 @@
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24" t="s">
+      <c r="I3" s="16"/>
+      <c r="J3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="24"/>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="J5" s="25" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="24"/>
-    </row>
-    <row r="7" spans="1:13" ht="36" x14ac:dyDescent="0.25">
-      <c r="C7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="C8" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="19">
-        <v>0</v>
-      </c>
-      <c r="E9" s="19">
-        <v>0</v>
-      </c>
-      <c r="F9" s="19">
-        <v>0</v>
-      </c>
+      <c r="K5" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:F9"/>
+  <mergeCells count="6">
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="H3:I3"/>
@@ -1169,54 +990,54 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="N1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="T1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>41</v>
+      <c r="B2" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1224,29 +1045,29 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+        <v>23</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="N3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="T3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1254,25 +1075,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="T4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1280,25 +1101,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="N5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="Q5" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="T5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1306,22 +1127,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="Q6" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="T6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1329,19 +1150,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="Q7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1349,57 +1170,57 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="N8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="N9" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>16</v>
+      <c r="B17" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
-        <v>21</v>
+      <c r="B18" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>26</v>
+      <c r="B19" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>29</v>
+      <c r="B20" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>59</v>
+      <c r="B21" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
-        <v>63</v>
+      <c r="B22" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished with format excelSmeta.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB55BC7-C06D-4A70-9B67-693F34069FAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E05B5-F77E-434E-A8CF-CB5160A8AA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="495" windowWidth="16440" windowHeight="16215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -855,7 +855,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Create discountForm.To be continued.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E05B5-F77E-434E-A8CF-CB5160A8AA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED8BFB9-DC83-4AE5-B2E9-2A8B65E505CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="3120" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
     <sheet name="Serv" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Cмета проекта</t>
   </si>
@@ -47,9 +47,48 @@
     <t>Световое оборудование/Lighting equipment</t>
   </si>
   <si>
+    <t>Наименование, name</t>
+  </si>
+  <si>
+    <t>Кол-во всего, qtt</t>
+  </si>
+  <si>
+    <t>Вес, weight</t>
+  </si>
+  <si>
+    <t>Мощность, power</t>
+  </si>
+  <si>
+    <t>Вес общ, weight total</t>
+  </si>
+  <si>
+    <t>заказанное кол-во, to take</t>
+  </si>
+  <si>
+    <t>Резерв</t>
+  </si>
+  <si>
+    <t>аренда 1 прибора, price per unit</t>
+  </si>
+  <si>
+    <t>Стоимость общая, total cost</t>
+  </si>
+  <si>
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>Clay Paky Axcor beam 300</t>
+  </si>
+  <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightlink HD 1.9 0.4x0.3m,  208x156 pixel, 0.12 sq m</t>
+  </si>
+  <si>
     <t>id_Dep</t>
   </si>
   <si>
@@ -77,9 +116,6 @@
     <t>---</t>
   </si>
   <si>
-    <t>Screen modules / Модупи экраны</t>
-  </si>
-  <si>
     <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
   </si>
   <si>
@@ -108,9 +144,6 @@
   </si>
   <si>
     <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>Экраны, медиасервера / Screens, mediaservers</t>
   </si>
   <si>
     <t>Пары, блайндера/PAR's, blinders</t>
@@ -204,7 +237,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +280,81 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF6600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +367,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F5F5" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99" tint="0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -339,87 +461,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC8C8DC" tint="0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC8C8DC" tint="0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC8C8DC" tint="0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC8C8DC" tint="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+  <cellXfs count="53">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="2">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="4" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="5" applyBorder="1" xfId="1" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" quotePrefix="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="2" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="4" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="4" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="6" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="7" applyFont="1" fillId="4" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="11" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="4" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="7" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Обычный 2" xfId="2"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -852,110 +1081,251 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.140625" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="12" width="12.5703125" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="C2" s="13" t="s">
+    <row r="1" ht="15.75">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" ht="26.25">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="14" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+    </row>
+    <row r="3" ht="15.75">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="17" t="s">
+      <c r="I3" s="18"/>
+      <c r="J3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="17"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="11" t="s">
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" ht="15.75">
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" ht="15.75">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="18" t="s">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="17"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="7">
+      <c r="C7" s="38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" ht="36" customHeight="1" s="39" customFormat="1">
+      <c r="C8" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" s="46" customFormat="1">
+      <c r="C10" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="48">
+        <v>128</v>
+      </c>
+      <c r="E10" s="48">
+        <v>16</v>
+      </c>
+      <c r="F10" s="48">
+        <v>350</v>
+      </c>
+      <c r="G10" s="49">
+        <v>16</v>
+      </c>
+      <c r="H10" s="50">
+        <v>1</v>
+      </c>
+      <c r="I10" s="51">
+        <v>0</v>
+      </c>
+      <c r="J10" s="52">
+        <v>80</v>
+      </c>
+      <c r="K10" s="52">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" ht="36" customHeight="1" s="24" customFormat="1">
+      <c r="C17" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" s="31" customFormat="1">
+      <c r="C19" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="33">
+        <v>70</v>
+      </c>
+      <c r="E19" s="33">
+        <v>4</v>
+      </c>
+      <c r="F19" s="33">
+        <v>180</v>
+      </c>
+      <c r="G19" s="34">
+        <v>4</v>
+      </c>
+      <c r="H19" s="35">
+        <v>1</v>
+      </c>
+      <c r="I19" s="36">
+        <v>0</v>
+      </c>
+      <c r="J19" s="37">
+        <v>90</v>
+      </c>
+      <c r="K19" s="37">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="D5:G5"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:F9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:G5" xr:uid="{40F0A1AB-4457-4065-A182-F6C4E68A1A9D}">
@@ -964,6 +1334,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -979,252 +1350,253 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
-    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="97.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="66" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="62" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="67.5703125" customWidth="1"/>
+    <col min="11" max="11" bestFit="1" width="60.42578125" customWidth="1"/>
+    <col min="14" max="14" bestFit="1" width="60.140625" customWidth="1"/>
+    <col min="17" max="17" bestFit="1" width="97.42578125" customWidth="1"/>
+    <col min="20" max="20" bestFit="1" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="H2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="E9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" ht="21">
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="N6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" t="s">
+    </row>
+    <row r="18" ht="21">
+      <c r="B18" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" ht="21">
+      <c r="B19" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-      <c r="N7" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="20" ht="21">
+      <c r="B20" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="N9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>53</v>
+    </row>
+    <row r="21" ht="21">
+      <c r="B21" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" ht="21">
+      <c r="B22" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Making summary and discount.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC459D87-1B53-4F82-AD9A-029AE4B3FEEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A650E5DE-F8F9-4F9B-96DA-F383F85C2038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="0" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -50,88 +50,88 @@
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
     <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
   </si>
   <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
+    <t>Коммутация/Commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
+    <t>Пары, блайндера/PAR's, blinders</t>
+  </si>
+  <si>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
+  </si>
+  <si>
+    <t>Мониторы / monitors</t>
+  </si>
+  <si>
     <t>Коммутация / Commutation</t>
-  </si>
-  <si>
-    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
-  </si>
-  <si>
-    <t>Коммутация/Commutation</t>
-  </si>
-  <si>
-    <t>id_Dep</t>
-  </si>
-  <si>
-    <t>Dep_Name</t>
-  </si>
-  <si>
-    <t>id_Dep_1</t>
-  </si>
-  <si>
-    <t>id_Dep_2</t>
-  </si>
-  <si>
-    <t>id_Dep_3</t>
-  </si>
-  <si>
-    <t>id_Dep_4</t>
-  </si>
-  <si>
-    <t>id_Dep_5</t>
-  </si>
-  <si>
-    <t>id_Dep_6</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Screen modules / Модупи экраны</t>
-  </si>
-  <si>
-    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
-  </si>
-  <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
-    <t>Акустические системы / speakers</t>
-  </si>
-  <si>
-    <t>Media servers / Медиасервера</t>
-  </si>
-  <si>
-    <t>Фермы/truss 40x40</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
-  </si>
-  <si>
-    <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>Экраны, медиасервера / Screens, mediaservers</t>
-  </si>
-  <si>
-    <t>Пары, блайндера/PAR's, blinders</t>
-  </si>
-  <si>
-    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
-  </si>
-  <si>
-    <t>Силовая коммутация/power commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
-  </si>
-  <si>
-    <t>Мониторы / monitors</t>
   </si>
   <si>
     <t>Архитектурный свет/Architecture fixtures</t>
@@ -855,12 +855,13 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A15" sqref="A7:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="66.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -990,28 +991,28 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1019,25 +1020,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,24 +1051,24 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>28</v>
-      </c>
-      <c r="T3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,25 +1076,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>35</v>
-      </c>
-      <c r="T4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1101,13 +1102,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
         <v>38</v>
@@ -1200,12 +1201,12 @@
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Still working with summary and discount
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A650E5DE-F8F9-4F9B-96DA-F383F85C2038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF09F736-B383-4857-A29A-62B1351767BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="0" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="600" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -50,6 +50,27 @@
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>Пары, блайндера/PAR's, blinders</t>
+  </si>
+  <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t>Коммутация / Commutation</t>
+  </si>
+  <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>Конструктив</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
     <t>id_Dep</t>
   </si>
   <si>
@@ -77,18 +98,9 @@
     <t>---</t>
   </si>
   <si>
-    <t>Screen modules / Модупи экраны</t>
-  </si>
-  <si>
-    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
-  </si>
-  <si>
     <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
   </si>
   <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
     <t>Акустические системы / speakers</t>
   </si>
   <si>
@@ -110,12 +122,6 @@
     <t>Усилители / amp racks</t>
   </si>
   <si>
-    <t>Экраны, медиасервера / Screens, mediaservers</t>
-  </si>
-  <si>
-    <t>Пары, блайндера/PAR's, blinders</t>
-  </si>
-  <si>
     <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
   </si>
   <si>
@@ -131,9 +137,6 @@
     <t>Мониторы / monitors</t>
   </si>
   <si>
-    <t>Коммутация / Commutation</t>
-  </si>
-  <si>
     <t>Архитектурный свет/Architecture fixtures</t>
   </si>
   <si>
@@ -165,9 +168,6 @@
   </si>
   <si>
     <t>dj-оборудование / dj equipment</t>
-  </si>
-  <si>
-    <t>Конструктив</t>
   </si>
   <si>
     <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
@@ -855,7 +855,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A15" sqref="A7:XFD15"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,28 +991,28 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="N1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="T1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1020,25 +1020,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="T2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,24 +1051,24 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="Q3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,25 +1076,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1102,25 +1102,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1128,22 +1128,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Q6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="T6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
@@ -1201,22 +1201,22 @@
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished with Summary.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF09F736-B383-4857-A29A-62B1351767BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9258724-C5D4-4BE7-8A75-F5476979F043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="600" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="600" windowWidth="18270" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -50,6 +50,9 @@
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
+  </si>
+  <si>
     <t>Пары, блайндера/PAR's, blinders</t>
   </si>
   <si>
@@ -59,115 +62,112 @@
     <t>Screen modules / Модупи экраны</t>
   </si>
   <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
+    <t>Фермы. Моторы</t>
+  </si>
+  <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
+    <t>Коммутация/Commutation</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
+  </si>
+  <si>
+    <t>Мониторы / monitors</t>
+  </si>
+  <si>
     <t>Коммутация / Commutation</t>
   </si>
   <si>
-    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+    <t>Архитектурный свет/Architecture fixtures</t>
+  </si>
+  <si>
+    <t>Прочее/rest equipment</t>
+  </si>
+  <si>
+    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
+  </si>
+  <si>
+    <t>Микшерные пульты / mixing desks</t>
+  </si>
+  <si>
+    <t>Светодиодные приборы/LED fixtures</t>
+  </si>
+  <si>
+    <t>Проектора и проекционные экраны / Projectors and screens</t>
+  </si>
+  <si>
+    <t>Оборудование для подвесса/Rigging stuff</t>
+  </si>
+  <si>
+    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
+  </si>
+  <si>
+    <t>dj-оборудование / dj equipment</t>
   </si>
   <si>
     <t>Конструктив</t>
-  </si>
-  <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
-    <t>id_Dep</t>
-  </si>
-  <si>
-    <t>Dep_Name</t>
-  </si>
-  <si>
-    <t>id_Dep_1</t>
-  </si>
-  <si>
-    <t>id_Dep_2</t>
-  </si>
-  <si>
-    <t>id_Dep_3</t>
-  </si>
-  <si>
-    <t>id_Dep_4</t>
-  </si>
-  <si>
-    <t>id_Dep_5</t>
-  </si>
-  <si>
-    <t>id_Dep_6</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
-  </si>
-  <si>
-    <t>Акустические системы / speakers</t>
-  </si>
-  <si>
-    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
-  </si>
-  <si>
-    <t>Media servers / Медиасервера</t>
-  </si>
-  <si>
-    <t>Коммутация/Commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 40x40</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
-  </si>
-  <si>
-    <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
-  </si>
-  <si>
-    <t>Силовая коммутация/power commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
-  </si>
-  <si>
-    <t>Мониторы / monitors</t>
-  </si>
-  <si>
-    <t>Архитектурный свет/Architecture fixtures</t>
-  </si>
-  <si>
-    <t>Прочее/rest equipment</t>
-  </si>
-  <si>
-    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
-  </si>
-  <si>
-    <t>Микшерные пульты / mixing desks</t>
-  </si>
-  <si>
-    <t>Фермы. Моторы</t>
-  </si>
-  <si>
-    <t>Светодиодные приборы/LED fixtures</t>
-  </si>
-  <si>
-    <t>Проектора и проекционные экраны / Projectors and screens</t>
-  </si>
-  <si>
-    <t>Оборудование для подвесса/Rigging stuff</t>
-  </si>
-  <si>
-    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
-  </si>
-  <si>
-    <t>dj-оборудование / dj equipment</t>
   </si>
   <si>
     <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
@@ -855,7 +855,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,28 +991,28 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1020,25 +1020,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="Q2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="T2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,24 +1051,24 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K3" t="s">
         <v>29</v>
       </c>
       <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>31</v>
-      </c>
-      <c r="T3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,25 +1076,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
       <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>34</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>36</v>
-      </c>
-      <c r="T4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1102,13 +1102,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
         <v>39</v>
@@ -1128,22 +1128,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>44</v>
       </c>
-      <c r="H6" t="s">
+      <c r="N6" t="s">
         <v>45</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="T6" t="s">
         <v>47</v>
-      </c>
-      <c r="T6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
@@ -1201,22 +1201,22 @@
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished with discount and summary.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9258724-C5D4-4BE7-8A75-F5476979F043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935B4A62-4F66-410F-89E4-E0FF6FBDD5E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="600" windowWidth="18270" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9045" yWindow="840" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -50,108 +50,114 @@
     <t>Головы/Moving heads</t>
   </si>
   <si>
+    <t>Экраны, медиасервера / Screens, mediaservers</t>
+  </si>
+  <si>
+    <t>Screen modules / Модупи экраны</t>
+  </si>
+  <si>
+    <t>Коммутация / Commutation</t>
+  </si>
+  <si>
+    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
+  </si>
+  <si>
+    <t>Коммутация/Commutation</t>
+  </si>
+  <si>
+    <t>Звуковое оборудование / Sound equipment</t>
+  </si>
+  <si>
+    <t>Мониторы / monitors</t>
+  </si>
+  <si>
+    <t>Микшерные пульты / mixing desks</t>
+  </si>
+  <si>
+    <t>dj-оборудование / dj equipment</t>
+  </si>
+  <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
     <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
   </si>
   <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
     <t>Пары, блайндера/PAR's, blinders</t>
   </si>
   <si>
-    <t>Экраны, медиасервера / Screens, mediaservers</t>
-  </si>
-  <si>
-    <t>Screen modules / Модупи экраны</t>
-  </si>
-  <si>
-    <t>Media servers / Медиасервера</t>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
+  </si>
+  <si>
+    <t>Архитектурный свет/Architecture fixtures</t>
+  </si>
+  <si>
+    <t>Прочее/rest equipment</t>
+  </si>
+  <si>
+    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
   </si>
   <si>
     <t>Фермы. Моторы</t>
   </si>
   <si>
-    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
-  </si>
-  <si>
-    <t>Фермы/truss 40x40</t>
-  </si>
-  <si>
-    <t>id_Dep</t>
-  </si>
-  <si>
-    <t>Dep_Name</t>
-  </si>
-  <si>
-    <t>id_Dep_1</t>
-  </si>
-  <si>
-    <t>id_Dep_2</t>
-  </si>
-  <si>
-    <t>id_Dep_3</t>
-  </si>
-  <si>
-    <t>id_Dep_4</t>
-  </si>
-  <si>
-    <t>id_Dep_5</t>
-  </si>
-  <si>
-    <t>id_Dep_6</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
-  </si>
-  <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
-    <t>Акустические системы / speakers</t>
-  </si>
-  <si>
-    <t>Коммутация/Commutation</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
-  </si>
-  <si>
-    <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
-  </si>
-  <si>
-    <t>Силовая коммутация/power commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
-  </si>
-  <si>
-    <t>Мониторы / monitors</t>
-  </si>
-  <si>
-    <t>Коммутация / Commutation</t>
-  </si>
-  <si>
-    <t>Архитектурный свет/Architecture fixtures</t>
-  </si>
-  <si>
-    <t>Прочее/rest equipment</t>
-  </si>
-  <si>
-    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
-  </si>
-  <si>
-    <t>Микшерные пульты / mixing desks</t>
-  </si>
-  <si>
     <t>Светодиодные приборы/LED fixtures</t>
   </si>
   <si>
@@ -164,9 +170,6 @@
     <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
   </si>
   <si>
-    <t>dj-оборудование / dj equipment</t>
-  </si>
-  <si>
     <t>Конструктив</t>
   </si>
   <si>
@@ -180,9 +183,6 @@
   </si>
   <si>
     <t>Разное / different details</t>
-  </si>
-  <si>
-    <t>Звуковое оборудование / Sound equipment</t>
   </si>
   <si>
     <t>Пульты/lighting desks</t>
@@ -855,7 +855,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,28 +991,28 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1020,25 +1020,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,24 +1051,24 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
       <c r="N3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="T3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,25 +1076,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="N4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="T4" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1102,25 +1102,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Q5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1128,22 +1128,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="T6" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1151,19 +1151,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -1201,27 +1201,27 @@
     </row>
     <row r="18" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished with discount and currency.Status OK
</commit_message>
<xml_diff>
--- a/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
+++ b/bin/Debug/datafolder/Smeta/SmetaTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935B4A62-4F66-410F-89E4-E0FF6FBDD5E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BF5A37-1906-4158-979E-207B13A4016E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9045" yWindow="840" windowWidth="17025" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Smeta" sheetId="1" r:id="rId1"/>
@@ -62,115 +62,115 @@
     <t>Силовые ящики, Димерные блоки/Power distribution, dimmers</t>
   </si>
   <si>
+    <t>Фермы. Моторы</t>
+  </si>
+  <si>
+    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
+  </si>
+  <si>
+    <t>Конструктив</t>
+  </si>
+  <si>
+    <t>СЦЕНА модули/stage modules</t>
+  </si>
+  <si>
+    <t>Звуковое оборудование / Sound equipment</t>
+  </si>
+  <si>
+    <t>Акустические системы / speakers</t>
+  </si>
+  <si>
+    <t>id_Dep</t>
+  </si>
+  <si>
+    <t>Dep_Name</t>
+  </si>
+  <si>
+    <t>id_Dep_1</t>
+  </si>
+  <si>
+    <t>id_Dep_2</t>
+  </si>
+  <si>
+    <t>id_Dep_3</t>
+  </si>
+  <si>
+    <t>id_Dep_4</t>
+  </si>
+  <si>
+    <t>id_Dep_5</t>
+  </si>
+  <si>
+    <t>id_Dep_6</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
+  </si>
+  <si>
+    <t>Media servers / Медиасервера</t>
+  </si>
+  <si>
     <t>Коммутация/Commutation</t>
   </si>
   <si>
-    <t>Звуковое оборудование / Sound equipment</t>
+    <t>Фермы/truss 40x40</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
+  </si>
+  <si>
+    <t>Усилители / amp racks</t>
+  </si>
+  <si>
+    <t>Пары, блайндера/PAR's, blinders</t>
+  </si>
+  <si>
+    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
+  </si>
+  <si>
+    <t>Силовая коммутация/power commutation</t>
+  </si>
+  <si>
+    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
   </si>
   <si>
     <t>Мониторы / monitors</t>
   </si>
   <si>
+    <t>Архитектурный свет/Architecture fixtures</t>
+  </si>
+  <si>
+    <t>Прочее/rest equipment</t>
+  </si>
+  <si>
+    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
+  </si>
+  <si>
+    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
+  </si>
+  <si>
     <t>Микшерные пульты / mixing desks</t>
   </si>
   <si>
+    <t>Светодиодные приборы/LED fixtures</t>
+  </si>
+  <si>
+    <t>Проектора и проекционные экраны / Projectors and screens</t>
+  </si>
+  <si>
+    <t>Оборудование для подвесса/Rigging stuff</t>
+  </si>
+  <si>
+    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
+  </si>
+  <si>
     <t>dj-оборудование / dj equipment</t>
-  </si>
-  <si>
-    <t>id_Dep</t>
-  </si>
-  <si>
-    <t>Dep_Name</t>
-  </si>
-  <si>
-    <t>id_Dep_1</t>
-  </si>
-  <si>
-    <t>id_Dep_2</t>
-  </si>
-  <si>
-    <t>id_Dep_3</t>
-  </si>
-  <si>
-    <t>id_Dep_4</t>
-  </si>
-  <si>
-    <t>id_Dep_5</t>
-  </si>
-  <si>
-    <t>id_Dep_6</t>
-  </si>
-  <si>
-    <t>---</t>
-  </si>
-  <si>
-    <t>Фермы/ truss 30x30, Фермы/ truss 40x40</t>
-  </si>
-  <si>
-    <t>СЦЕНА модули/stage modules</t>
-  </si>
-  <si>
-    <t>Акустические системы / speakers</t>
-  </si>
-  <si>
-    <t>Стробоскопы/strobes, Прожектора следящего света/followspots</t>
-  </si>
-  <si>
-    <t>Media servers / Медиасервера</t>
-  </si>
-  <si>
-    <t>Фермы/truss 40x40</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Основания / Foot / J001, Удлиннители / Expander / J002, Вертикальные ноги / legs / J003</t>
-  </si>
-  <si>
-    <t>Усилители / amp racks</t>
-  </si>
-  <si>
-    <t>Пары, блайндера/PAR's, blinders</t>
-  </si>
-  <si>
-    <t>Controllers, convertors and rest / Контроллеры, преобразователи и др</t>
-  </si>
-  <si>
-    <t>Силовая коммутация/power commutation</t>
-  </si>
-  <si>
-    <t>Фермы/truss 50x60, Фермы/truss 52x52</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, горизонтальные ригели / rigel / J004, Откосы / diagonal / J005</t>
-  </si>
-  <si>
-    <t>Архитектурный свет/Architecture fixtures</t>
-  </si>
-  <si>
-    <t>Прочее/rest equipment</t>
-  </si>
-  <si>
-    <t>Лебедки, лебедочные контроллеры/motors, motor controllers</t>
-  </si>
-  <si>
-    <t>ЛЕСА/Scaffold, Откосы / diagonal / J005, лестницы / Steps, Клыки сцены / claws, Платформы / plarform</t>
-  </si>
-  <si>
-    <t>Фермы. Моторы</t>
-  </si>
-  <si>
-    <t>Светодиодные приборы/LED fixtures</t>
-  </si>
-  <si>
-    <t>Проектора и проекционные экраны / Projectors and screens</t>
-  </si>
-  <si>
-    <t>Оборудование для подвесса/Rigging stuff</t>
-  </si>
-  <si>
-    <t>Барьеры/barricades, Разное / different details, Тенты / canvas</t>
-  </si>
-  <si>
-    <t>Конструктив</t>
   </si>
   <si>
     <t>Дым, туман, вентиляторы, прочее/Fog, Haze, fans, rest</t>
@@ -855,7 +855,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,28 +991,28 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1032,13 +1032,13 @@
         <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,24 +1051,24 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
         <v>31</v>
       </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>33</v>
-      </c>
-      <c r="T3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,22 +1079,22 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
         <v>35</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>36</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>37</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>39</v>
-      </c>
-      <c r="T4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
         <v>41</v>
@@ -1120,7 +1120,7 @@
         <v>43</v>
       </c>
       <c r="T5" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1128,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>45</v>
@@ -1143,7 +1143,7 @@
         <v>48</v>
       </c>
       <c r="T6" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>50</v>
@@ -1171,7 +1171,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
         <v>54</v>
@@ -1211,17 +1211,17 @@
     </row>
     <row r="20" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="21" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>